<commit_message>
Changed the read uncommitted data to serializable data
</commit_message>
<xml_diff>
--- a/dbq5data.xlsx
+++ b/dbq5data.xlsx
@@ -22,148 +22,148 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
+    <t xml:space="preserve">['question5.py', 'READ COMMITTED']</t>
+  </si>
+  <si>
     <t xml:space="preserve">['question5.py', 'REPEATABLE READ']</t>
   </si>
   <si>
-    <t xml:space="preserve">['question5.py', 'READ COMMITTED']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['question5.py', 'READ UNCOMMITTED']</t>
+    <t xml:space="preserve">['question5.py', 'SERIALIZABLE']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S: 500, E: 2500, T: 1, I: READ COMMITTED</t>
   </si>
   <si>
     <t xml:space="preserve">S: 500, E: 2500, T: 1, I: REPEATABLE READ</t>
   </si>
   <si>
-    <t xml:space="preserve">S: 500, E: 2500, T: 1, I: READ COMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S: 500, E: 2500, T: 1, I: READ UNCOMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 8.697224 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 18.995593 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 10.969793 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 28.026985 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 21.639499 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 23.071385 time to finish</t>
+    <t xml:space="preserve">S: 500, E: 2500, T: 1, I: SERIALIZABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 23.703131 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 29.040507 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 29.437218 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 12.888935 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.584639 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.574540 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S: 500, E: 500, T: 5, I: READ COMMITTED</t>
   </si>
   <si>
     <t xml:space="preserve">S: 500, E: 500, T: 5, I: REPEATABLE READ</t>
   </si>
   <si>
-    <t xml:space="preserve">S: 500, E: 500, T: 5, I: READ COMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S: 500, E: 500, T: 5, I: READ UNCOMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 8.163739 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 18.841333 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 9.765552 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 11.846126 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 12.554905 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 10.467679 time to finish</t>
+    <t xml:space="preserve">S: 500, E: 500, T: 5, I: SERIALIZABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 11.108206 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 13.401326 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 12.038902 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 13.054464 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.691852 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.593463 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S: 500, E: 250, T: 10, I: READ COMMITTED</t>
   </si>
   <si>
     <t xml:space="preserve">S: 500, E: 250, T: 10, I: REPEATABLE READ</t>
   </si>
   <si>
-    <t xml:space="preserve">S: 500, E: 250, T: 10, I: READ COMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S: 500, E: 250, T: 10, I: READ UNCOMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 8.559783 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 18.504623 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 10.002508 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 10.521229 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 8.687495 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 8.884444 time to finish</t>
+    <t xml:space="preserve">S: 500, E: 250, T: 10, I: SERIALIZABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 6.279267 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 10.347166 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 10.402270 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 12.898454 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.460448 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.481740 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S: 500, E: 100, T: 25, I: READ COMMITTED</t>
   </si>
   <si>
     <t xml:space="preserve">S: 500, E: 100, T: 25, I: REPEATABLE READ</t>
   </si>
   <si>
-    <t xml:space="preserve">S: 500, E: 100, T: 25, I: READ COMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S: 500, E: 100, T: 25, I: READ UNCOMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 8.303914 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 18.603799 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 10.003635 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 9.583558 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 4.421148 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 4.120228 time to finish</t>
+    <t xml:space="preserve">S: 500, E: 100, T: 25, I: SERIALIZABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 4.085643 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 9.829875 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 9.825487 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 13.264877 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.449010 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.502322 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S: 500, E: 50, T: 50, I: READ COMMITTED</t>
   </si>
   <si>
     <t xml:space="preserve">S: 500, E: 50, T: 50, I: REPEATABLE READ</t>
   </si>
   <si>
-    <t xml:space="preserve">S: 500, E: 50, T: 50, I: READ COMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S: 500, E: 50, T: 50, I: READ UNCOMMITTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 8.462903 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 18.869834 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_isolation took 9.794858 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 9.652873 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 2.829239 time to finish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run_exchanges took 2.500674 time to finish</t>
+    <t xml:space="preserve">S: 500, E: 50, T: 50, I: SERIALIZABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 3.122220 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 10.085353 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_exchanges took 9.887863 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 13.888793 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.873881 time to finish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_isolation took 8.454599 time to finish</t>
   </si>
 </sst>
 </file>
@@ -262,7 +262,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>